<commit_message>
script para inserir dados nas tabelas do postgres
</commit_message>
<xml_diff>
--- a/dados/exemplo_amostra.xlsx
+++ b/dados/exemplo_amostra.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/770c1f2889b1c44a/projetos_dados/visualizacao__de_dados/1 - Airbnb-analytics-dw/dados/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="347" documentId="11_1B4930B2D37053389BDB2311595ED87656C0C4F5" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{0DDB469F-C31E-42BB-9EA1-7CF95CE16CC9}"/>
+  <xr:revisionPtr revIDLastSave="443" documentId="11_1B4930B2D37053389BDB2311595ED87656C0C4F5" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D464AE40-6335-4933-BF55-41D1BBD99B8E}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -7234,9 +7234,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:CS101"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="23.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -32233,7 +32231,6 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:CS101" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
@@ -32243,7 +32240,7 @@
   <dimension ref="A1:D115"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A21" sqref="A21:XFD21"/>
+      <selection activeCell="C40" sqref="C40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>